<commit_message>
vc-5 feature/add creadit and whitelisting
</commit_message>
<xml_diff>
--- a/obdUploads/data.xlsx
+++ b/obdUploads/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,42 +409,107 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>9799972372</v>
+        <v>7014118238</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>6367772185</v>
+        <v>7075812222</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>9694601301</v>
+        <v>9885861677</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>78910 27888</v>
+        <v>9902459657</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>86964 62997</v>
+        <v>8970511445</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>76656 86352</v>
+        <v>9535114669</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>70141 18238</v>
+        <v>9901396041</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>9845704305</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>9164558164</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>9844329150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6363179872</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>9916725929</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>9481270887</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>7760493586</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>9448107102</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>9844060947</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>9663093906</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>9632535125</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>9480230542</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>9008150443</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vc-6 adding credit and cutting
</commit_message>
<xml_diff>
--- a/obdUploads/data.xlsx
+++ b/obdUploads/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,107 +409,32 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>7014118238</v>
+        <v>7075812222</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>7075812222</v>
+        <v>9885861677</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>9885861677</v>
+        <v>8341325077</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>9902459657</v>
+        <v>9640494242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>8970511445</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>9535114669</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>9901396041</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>9845704305</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>9164558164</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9844329150</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>6363179872</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>9916725929</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>9481270887</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>7760493586</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>9448107102</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>9844060947</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>9663093906</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>9632535125</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>9480230542</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>9008150443</v>
+        <v>7014118238</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>